<commit_message>
adding TC-04, TC-05, and update excel test case
</commit_message>
<xml_diff>
--- a/Documentation/miniproject - test case.xlsx
+++ b/Documentation/miniproject - test case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prasetyo Bintang\miniproject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C566702-3A02-45D8-B4E3-5E375101F684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA62E5-2158-4232-86B5-85CF95701DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{91CE409F-3903-42AA-824B-7B9D5348EDB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
   <si>
     <t>Title</t>
   </si>
@@ -235,6 +235,38 @@
 3. User mengisi password dengan dengan secret_sauce
 4. User klik tombol login
 5. Sistem validasi credential</t>
+  </si>
+  <si>
+    <t>TC-04</t>
+  </si>
+  <si>
+    <t>1. User membuka halaman saucedemo.com
+2. User tidak mengisi kolom username
+3. User mengisi password dengan secret_sauce
+4. User klik tombol login
+5. Sistem validasi credential</t>
+  </si>
+  <si>
+    <t>User gagal login dan muncul pesan error: 'Epic sadface: Username is required'</t>
+  </si>
+  <si>
+    <t>TC-05</t>
+  </si>
+  <si>
+    <t>User gagal login menggunakan username yang kosong dan password valid</t>
+  </si>
+  <si>
+    <t>User gagal login menggunakan username valid dan password yang kosong</t>
+  </si>
+  <si>
+    <t>1. User membuka halaman saucedemo.com
+2. User mengisi username dengan standard_user
+3. User tidak mengisi kolom password
+4. User klik tombol login
+5. Sistem validasi credential</t>
+  </si>
+  <si>
+    <t>User gagal login dan muncul pesan error: 'Epic sadface: Password is required'</t>
   </si>
 </sst>
 </file>
@@ -936,8 +968,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}" name="Table3" displayName="Table3" ref="A13:L17" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A13:L17" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}" name="Table3" displayName="Table3" ref="A13:L19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A13:L19" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{997C61E7-393A-48E0-AE62-AB52E8161F44}" name="Column1" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{1FAB5D1B-4DE2-46CD-919C-792226AEBE04}" name="Column2" dataDxfId="10"/>
@@ -1253,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1625EE-3359-4552-AA9B-297E0245A5A8}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,12 +1614,12 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
@@ -1605,14 +1637,78 @@
         <v>50</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modify script TC-01 - TC-05 and adding TC-06
</commit_message>
<xml_diff>
--- a/Documentation/miniproject - test case.xlsx
+++ b/Documentation/miniproject - test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prasetyo Bintang\miniproject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA62E5-2158-4232-86B5-85CF95701DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AE86DE-9E1B-42DA-A1D1-D00AA801FAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{91CE409F-3903-42AA-824B-7B9D5348EDB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>Title</t>
   </si>
@@ -267,6 +267,24 @@
   </si>
   <si>
     <t>User gagal login dan muncul pesan error: 'Epic sadface: Password is required'</t>
+  </si>
+  <si>
+    <t>TC-06</t>
+  </si>
+  <si>
+    <t>User gagal login menggunakan username dan password kosong</t>
+  </si>
+  <si>
+    <t>1. User membuka halaman saucedemo.com
+2. User tidak mengisi kolom username
+3. User tidak mengisi kolom password
+4. User klik tombol login
+5. Sistem validasi credential</t>
+  </si>
+  <si>
+    <t>1. Jika user tidak mengisi kedua field maka muncul pesan error: 'Epic sadface: Username is required'
+2. Jika user hanya mengisi username maka muncul pesan error: 'Epic sadface: Password is required'
+3. Jika user hanya mengisi password maka pesan error: 'Epic sadface: Username is required'</t>
   </si>
 </sst>
 </file>
@@ -968,8 +986,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}" name="Table3" displayName="Table3" ref="A13:L19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A13:L19" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}" name="Table3" displayName="Table3" ref="A13:L20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A13:L20" xr:uid="{5C89DF54-902F-46E5-9012-88B99A896097}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{997C61E7-393A-48E0-AE62-AB52E8161F44}" name="Column1" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{1FAB5D1B-4DE2-46CD-919C-792226AEBE04}" name="Column2" dataDxfId="10"/>
@@ -1285,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1625EE-3359-4552-AA9B-297E0245A5A8}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,11 +1317,12 @@
     <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12" style="1" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1678,12 +1697,12 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
@@ -1701,14 +1720,46 @@
         <v>50</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>